<commit_message>
Attached files for last commit
I've forgot to attach files for the last commit
</commit_message>
<xml_diff>
--- a/SL_Intelligent_Room/Output/SLDLL_relay/frequencies.xlsx
+++ b/SL_Intelligent_Room/Output/SLDLL_relay/frequencies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\info\repo\dzkbx0_thesis_repo\SL_Intelligent_Room\Output\SLDLL_relay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1409A26-23E7-4FA0-B31D-03C683D013D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B5DA1F-9DF9-43C0-BA3E-EB109FB178DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1065" yWindow="-120" windowWidth="27855" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -697,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A106A306-3212-45AE-B471-21B6B5618BDF}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>